<commit_message>
Load records for pivot tables into XLPivotTableCache. Doesn't write them out yet.
The modified test fiels contained values for a shared items in a table the definition shouldn't contains (e.g. pure numeric values not found in original table definition).
</commit_message>
<xml_diff>
--- a/ClosedXML.Tests/Resource/Other/PivotTableReferenceFiles/PivotSubtotalsSource/output.xlsx
+++ b/ClosedXML.Tests/Resource/Other/PivotTableReferenceFiles/PivotSubtotalsSource/output.xlsx
@@ -514,20 +514,10 @@
       </x:sharedItems>
     </x:cacheField>
     <x:cacheField name="Ship date">
-      <x:sharedItems containsSemiMixedTypes="0" containsNonDate="0" containsDate="1" containsString="0" minDate="1988-05-26T00:00:00" maxDate="1993-10-19T00:00:00" count="4">
-        <x:d v="1988-05-26T00:00:00"/>
-        <x:d v="1988-07-19T00:00:00"/>
-        <x:d v="1988-08-27T00:00:00"/>
-        <x:d v="1993-10-19T00:00:00"/>
-      </x:sharedItems>
+      <x:sharedItems/>
     </x:cacheField>
     <x:cacheField name="Items total">
-      <x:sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="134.85" maxValue="20108" count="4">
-        <x:n v="134.85"/>
-        <x:n v="20108"/>
-        <x:n v="10152"/>
-        <x:n v="1004.8"/>
-      </x:sharedItems>
+      <x:sharedItems/>
     </x:cacheField>
     <x:cacheField name="Tax rate">
       <x:sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="0" maxValue="0" count="1">
@@ -535,12 +525,7 @@
       </x:sharedItems>
     </x:cacheField>
     <x:cacheField name="Amount paid">
-      <x:sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="134.85" maxValue="20108" count="4">
-        <x:n v="134.85"/>
-        <x:n v="20108"/>
-        <x:n v="10152"/>
-        <x:n v="1004.8"/>
-      </x:sharedItems>
+      <x:sharedItems/>
     </x:cacheField>
   </x:cacheFields>
   <x:extLst>

</xml_diff>

<commit_message>
Add statistics to pivot cache field.
Field statistics are stored in the file and are available, even if field has no records (save source data = false). Ensure the values are propertly loaded/updated with record values and saved back.

The statistics are not very useful for ClosedXML, but Excel likely uses them for optimized loadings and field structure.
</commit_message>
<xml_diff>
--- a/ClosedXML.Tests/Resource/Other/PivotTableReferenceFiles/PivotSubtotalsSource/output.xlsx
+++ b/ClosedXML.Tests/Resource/Other/PivotTableReferenceFiles/PivotSubtotalsSource/output.xlsx
@@ -514,10 +514,10 @@
       </x:sharedItems>
     </x:cacheField>
     <x:cacheField name="Ship date">
-      <x:sharedItems/>
+      <x:sharedItems containsSemiMixedTypes="0" containsNonDate="0" containsDate="1" containsString="0" minDate="1988-05-26T00:00:00" maxDate="1993-10-20T00:00:00"/>
     </x:cacheField>
     <x:cacheField name="Items total">
-      <x:sharedItems/>
+      <x:sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="134.85" maxValue="20108"/>
     </x:cacheField>
     <x:cacheField name="Tax rate">
       <x:sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="0" maxValue="0" count="1">
@@ -525,7 +525,7 @@
       </x:sharedItems>
     </x:cacheField>
     <x:cacheField name="Amount paid">
-      <x:sharedItems/>
+      <x:sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="134.85" maxValue="20108"/>
     </x:cacheField>
   </x:cacheFields>
   <x:extLst>

</xml_diff>

<commit_message>
Add data fields structures through many methods are still not implemented.
PivotSubtotalsLoadingTest - Mostly styles has been fixed. PivotTable now references two styles
</commit_message>
<xml_diff>
--- a/ClosedXML.Tests/Resource/Other/PivotTableReferenceFiles/PivotSubtotalsSource/output.xlsx
+++ b/ClosedXML.Tests/Resource/Other/PivotTableReferenceFiles/PivotSubtotalsSource/output.xlsx
@@ -578,139 +578,132 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<x:pivotTableDefinition xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="0" dataCaption="Values" showError="0" missingCaption="" showMissing="1" pageWrap="0" pageOverThenDown="0" itemPrintTitles="1" mergeItem="1" indent="0" compact="0" compactData="0" gridDropZones="1">
-  <x:location ref="B3" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
-  <x:pivotFields count="7">
-    <x:pivotField name="Company" axis="axisRow" compact="0" outline="0" showAll="0" includeNewItemsInFilter="1">
-      <x:items count="2">
-        <x:item x="0"/>
-        <x:item t="default"/>
-      </x:items>
-    </x:pivotField>
-    <x:pivotField name="Payment method" axis="axisRow" compact="0" outline="0" showAll="0" includeNewItemsInFilter="1">
-      <x:items count="4">
-        <x:item x="0"/>
-        <x:item x="1"/>
-        <x:item x="2"/>
-        <x:item t="default"/>
-      </x:items>
-    </x:pivotField>
-    <x:pivotField name="OrderNo" axis="axisRow" compact="0" outline="0" showAll="0" includeNewItemsInFilter="1">
-      <x:items count="5">
-        <x:item x="0"/>
-        <x:item x="1"/>
-        <x:item x="2"/>
-        <x:item x="3"/>
-        <x:item t="default"/>
-      </x:items>
-    </x:pivotField>
-    <x:pivotField name="Ship date" compact="0" outline="0">
-      <x:items count="1">
-        <x:item t="default"/>
-      </x:items>
-    </x:pivotField>
-    <x:pivotField name="Items total" dataField="1" compact="0" outline="0">
-      <x:items count="1">
-        <x:item t="default"/>
-      </x:items>
-    </x:pivotField>
-    <x:pivotField name="Tax rate" axis="axisCol" compact="0" outline="0" showAll="0" includeNewItemsInFilter="1">
-      <x:items count="2">
-        <x:item x="0"/>
-        <x:item t="default"/>
-      </x:items>
-    </x:pivotField>
-    <x:pivotField name="Amount paid" dataField="1" compact="0" outline="0">
-      <x:items count="1">
-        <x:item t="default"/>
-      </x:items>
-    </x:pivotField>
-  </x:pivotFields>
-  <x:rowFields count="3">
-    <x:field x="0"/>
-    <x:field x="1"/>
-    <x:field x="2"/>
-  </x:rowFields>
-  <x:rowItems count="11">
-    <x:i>
-      <x:x v="0"/>
-    </x:i>
-    <x:i t="grand">
-      <x:x/>
-    </x:i>
-    <x:i>
-      <x:x v="0"/>
-    </x:i>
-    <x:i>
-      <x:x v="1"/>
-    </x:i>
-    <x:i>
-      <x:x v="2"/>
-    </x:i>
-    <x:i t="grand">
-      <x:x/>
-    </x:i>
-    <x:i>
-      <x:x v="0"/>
-    </x:i>
-    <x:i>
-      <x:x v="1"/>
-    </x:i>
-    <x:i>
-      <x:x v="2"/>
-    </x:i>
-    <x:i>
-      <x:x v="3"/>
-    </x:i>
-    <x:i t="grand">
-      <x:x/>
-    </x:i>
-  </x:rowItems>
-  <x:colFields count="2">
-    <x:field x="5"/>
-    <x:field x="-2"/>
-  </x:colFields>
-  <x:colItems count="2">
-    <x:i>
-      <x:x v="0"/>
-    </x:i>
-    <x:i t="grand">
-      <x:x/>
-    </x:i>
-  </x:colItems>
-  <x:dataFields count="2">
-    <x:dataField name="Sum Amount paid" fld="6" subtotal="sum" showDataAs="normal" baseField="3" baseItem="0" numFmtId="0"/>
-    <x:dataField name="Sum Items total" fld="4" subtotal="sum" showDataAs="normal" baseField="3" baseItem="0" numFmtId="0"/>
-  </x:dataFields>
-  <x:formats count="4">
-    <x:format dxfId="1">
-      <x:pivotArea type="normal" grandRow="1" axis="axisRow" fieldPosition="0"/>
-    </x:format>
-    <x:format dxfId="1">
-      <x:pivotArea type="normal" dataOnly="0" labelOnly="1" grandRow="1" axis="axisRow" fieldPosition="0"/>
-    </x:format>
-    <x:format dxfId="2">
-      <x:pivotArea type="normal" fieldPosition="0">
-        <x:references count="1">
-          <x:reference field="0" defaultSubtotal="1"/>
-        </x:references>
-      </x:pivotArea>
-    </x:format>
-    <x:format dxfId="2">
-      <x:pivotArea type="normal" dataOnly="0" labelOnly="1" fieldPosition="0">
-        <x:references count="1">
-          <x:reference field="5"/>
-        </x:references>
-      </x:pivotArea>
-    </x:format>
-  </x:formats>
-  <x:pivotTableStyleInfo showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0"/>
-  <x:extLst>
-    <x:ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" enableEdit="0" hideValuesRow="1"/>
-    </x:ext>
-  </x:extLst>
-</x:pivotTableDefinition>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0" dataCaption="Values" updatedVersion="8" itemPrintTitles="1" mergeItem="1" indent="0" compact="0" compactData="0" gridDropZones="1">
+  <location ref="B3:H14" firstHeaderRow="1" firstDataRow="3" firstDataCol="3"/>
+  <pivotFields count="7">
+    <pivotField name="Company" axis="axisRow" compact="0" outline="0" showAll="0" includeNewItemsInFilter="1">
+      <items count="2">
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField name="Payment method" axis="axisRow" compact="0" outline="0" showAll="0" includeNewItemsInFilter="1">
+      <items count="4">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField name="OrderNo" axis="axisRow" compact="0" outline="0" showAll="0" includeNewItemsInFilter="1">
+      <items count="5">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField name="Ship date" compact="0" outline="0"/>
+    <pivotField name="Items total" dataField="1" compact="0" outline="0"/>
+    <pivotField name="Tax rate" axis="axisCol" compact="0" outline="0" showAll="0" includeNewItemsInFilter="1">
+      <items count="2">
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField name="Amount paid" dataField="1" compact="0" outline="0"/>
+  </pivotFields>
+  <rowFields count="3">
+    <field x="0"/>
+    <field x="1"/>
+    <field x="2"/>
+  </rowFields>
+  <rowItems count="9">
+    <i>
+      <x/>
+      <x/>
+      <x/>
+    </i>
+    <i t="default" r="1">
+      <x/>
+    </i>
+    <i r="1">
+      <x v="1"/>
+      <x v="1"/>
+    </i>
+    <i r="2">
+      <x v="3"/>
+    </i>
+    <i t="default" r="1">
+      <x v="1"/>
+    </i>
+    <i r="1">
+      <x v="2"/>
+      <x v="2"/>
+    </i>
+    <i t="default" r="1">
+      <x v="2"/>
+    </i>
+    <i t="default">
+      <x/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="2">
+    <field x="5"/>
+    <field x="-2"/>
+  </colFields>
+  <colItems count="4">
+    <i>
+      <x/>
+      <x/>
+    </i>
+    <i r="1" i="1">
+      <x v="1"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+    <i t="grand" i="1">
+      <x/>
+    </i>
+  </colItems>
+  <dataFields count="2">
+    <dataField name="Sum Amount paid" fld="6" baseField="3" baseItem="0"/>
+    <dataField name="Sum Items total" fld="4" baseField="3" baseItem="0"/>
+  </dataFields>
+  <formats count="4">
+    <format dxfId="1">
+      <pivotArea grandRow="1" axis="axisRow" fieldPosition="0"/>
+    </format>
+    <format dxfId="1">
+      <pivotArea dataOnly="0" labelOnly="1" grandRow="1" axis="axisRow" fieldPosition="0"/>
+    </format>
+    <format dxfId="2">
+      <pivotArea fieldPosition="0">
+        <references count="1">
+          <reference field="0" count="0" defaultSubtotal="1"/>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="2">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="5" count="0"/>
+        </references>
+      </pivotArea>
+    </format>
+  </formats>
+  <pivotTableStyleInfo showRowHeaders="1" showColHeaders="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition enableEdit="0" hideValuesRow="1"/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>

</xml_diff>